<commit_message>
create common countries cleaning dict
</commit_message>
<xml_diff>
--- a/inst/extdata/cleaning_dictionary.xlsx
+++ b/inst/extdata/cleaning_dictionary.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aljc201/Desktop/covidmonitor/inst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spina\Desktop\covidmonitor\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9695C9EF-67ED-8A4C-B6D2-076FAFFD92D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="10680" windowWidth="34600" windowHeight="16060" xr2:uid="{057372D8-FD55-424B-B3E3-F97E8D1F1A18}"/>
+    <workbookView xWindow="10845" yWindow="10680" windowWidth="34605" windowHeight="16065" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="all_clean" sheetId="9" r:id="rId1"/>
     <sheet name="capital" sheetId="7" r:id="rId2"/>
     <sheet name="confirmed" sheetId="8" r:id="rId3"/>
+    <sheet name="country" sheetId="10" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="387">
   <si>
     <t>HYGIENE</t>
   </si>
@@ -1143,13 +1143,58 @@
   </si>
   <si>
     <t>sickle</t>
+  </si>
+  <si>
+    <t>COMORES</t>
+  </si>
+  <si>
+    <t>CÔTE D'IVOIRE</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>GABON</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>NIGER</t>
+  </si>
+  <si>
+    <t>République du Congo</t>
+  </si>
+  <si>
+    <t>SAO TOME ET PRINCIPE</t>
+  </si>
+  <si>
+    <t>SENEGAL</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Sao Tome &amp; Principe</t>
+  </si>
+  <si>
+    <t>Comores</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1523,20 +1568,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092CE1D0-0E52-5D44-9DBC-8794A4E177B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -1622,7 +1667,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1753,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1794,7 +1839,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1874,7 +1919,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1949,7 +1994,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2076,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2102,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2080,7 +2125,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2100,7 +2145,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2117,7 +2162,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2131,7 +2176,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2145,7 +2190,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2159,7 +2204,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2170,7 +2215,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2181,7 +2226,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2192,7 +2237,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2203,7 +2248,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2214,7 +2259,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2225,7 +2270,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2236,7 +2281,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2247,7 +2292,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2255,7 +2300,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -2263,7 +2308,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2271,7 +2316,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2279,7 +2324,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -2287,7 +2332,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -2295,7 +2340,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2303,7 +2348,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -2311,7 +2356,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2319,7 +2364,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -2327,252 +2372,252 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="28:28">
       <c r="AB33" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="28:28">
       <c r="AB34" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="28:28">
       <c r="AB35" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="28:28">
       <c r="AB36" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="28:28">
       <c r="AB37" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="28:28">
       <c r="AB38" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="28:28">
       <c r="AB39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="28:28">
       <c r="AB40" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="28:28">
       <c r="AB41" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="28:28">
       <c r="AB42" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="28:28">
       <c r="AB43" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="28:28">
       <c r="AB44" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="28:28">
       <c r="AB45" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="28:28">
       <c r="AB46" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="28:28">
       <c r="AB47" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="28:28">
       <c r="AB48" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="28:28">
       <c r="AB49" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="28:28">
       <c r="AB50" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="28:28">
       <c r="AB51" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="28:28">
       <c r="AB52" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="28:28">
       <c r="AB53" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="28:28">
       <c r="AB54" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="28:28">
       <c r="AB55" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="28:28">
       <c r="AB56" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="57" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="28:28">
       <c r="AB57" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="28:28">
       <c r="AB58" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="28:28">
       <c r="AB59" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="28:28">
       <c r="AB60" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="28:28">
       <c r="AB61" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="28:28">
       <c r="AB62" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="28:28">
       <c r="AB63" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="28:28">
       <c r="AB64" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="65" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="28:28">
       <c r="AB65" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="28:28">
       <c r="AB66" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="28:28">
       <c r="AB67" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="28:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="28:28" ht="15.75">
       <c r="AB68" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="69" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="28:28">
       <c r="AB69" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="28:28">
       <c r="AB70" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="28:28">
       <c r="AB71" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="28:28">
       <c r="AB72" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="73" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="28:28">
       <c r="AB73" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="74" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="28:28">
       <c r="AB74" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="75" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="28:28">
       <c r="AB75" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="28:28">
       <c r="AB76" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="28:28">
       <c r="AB77" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="78" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="28:28">
       <c r="AB78" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="28:28">
       <c r="AB79" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="28:28">
       <c r="AB80" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="81" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="81" spans="28:28">
       <c r="AB81" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="82" spans="28:28" x14ac:dyDescent="0.2">
+    <row r="82" spans="28:28">
       <c r="AB82" s="2" t="s">
         <v>349</v>
       </c>
@@ -2583,16 +2628,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8EFF2D-F821-E342-BE80-698EC0819BB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>233</v>
       </c>
@@ -2603,7 +2648,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>248</v>
       </c>
@@ -2614,7 +2659,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -2625,7 +2670,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>250</v>
       </c>
@@ -2636,7 +2681,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>265</v>
       </c>
@@ -2647,7 +2692,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -2658,7 +2703,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>251</v>
       </c>
@@ -2669,7 +2714,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -2680,7 +2725,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>267</v>
       </c>
@@ -2691,7 +2736,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>253</v>
       </c>
@@ -2702,7 +2747,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>253</v>
       </c>
@@ -2713,7 +2758,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>268</v>
       </c>
@@ -2724,7 +2769,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>269</v>
       </c>
@@ -2735,7 +2780,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>247</v>
       </c>
@@ -2746,7 +2791,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>246</v>
       </c>
@@ -2757,7 +2802,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>245</v>
       </c>
@@ -2768,7 +2813,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>270</v>
       </c>
@@ -2779,7 +2824,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>272</v>
       </c>
@@ -2790,7 +2835,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>271</v>
       </c>
@@ -2801,7 +2846,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>271</v>
       </c>
@@ -2812,7 +2857,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>273</v>
       </c>
@@ -2823,7 +2868,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>274</v>
       </c>
@@ -2834,7 +2879,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>320</v>
       </c>
@@ -2845,7 +2890,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>275</v>
       </c>
@@ -2857,7 +2902,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+  <sortState ref="A2:C24">
     <sortCondition ref="A1:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2865,16 +2910,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62F8E3E-3802-3F43-A0BC-8693C28A06B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>233</v>
       </c>
@@ -2888,7 +2933,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>304</v>
       </c>
@@ -2896,7 +2941,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>305</v>
       </c>
@@ -2904,7 +2949,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>248</v>
       </c>
@@ -2912,7 +2957,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>306</v>
       </c>
@@ -2920,7 +2965,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -2928,7 +2973,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -2936,7 +2981,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -2944,7 +2989,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>265</v>
       </c>
@@ -2958,7 +3003,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>308</v>
       </c>
@@ -2966,7 +3011,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>266</v>
       </c>
@@ -2974,7 +3019,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>309</v>
       </c>
@@ -2982,7 +3027,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>310</v>
       </c>
@@ -2990,7 +3035,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>251</v>
       </c>
@@ -2998,7 +3043,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>311</v>
       </c>
@@ -3006,7 +3051,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>312</v>
       </c>
@@ -3014,7 +3059,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>313</v>
       </c>
@@ -3022,7 +3067,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>252</v>
       </c>
@@ -3030,7 +3075,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>267</v>
       </c>
@@ -3038,7 +3083,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>314</v>
       </c>
@@ -3046,7 +3091,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>315</v>
       </c>
@@ -3054,7 +3099,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>268</v>
       </c>
@@ -3062,7 +3107,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>316</v>
       </c>
@@ -3070,7 +3115,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>269</v>
       </c>
@@ -3084,7 +3129,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="6" t="s">
         <v>247</v>
       </c>
@@ -3092,7 +3137,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>317</v>
       </c>
@@ -3100,7 +3145,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>246</v>
       </c>
@@ -3108,7 +3153,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>245</v>
       </c>
@@ -3116,7 +3161,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>270</v>
       </c>
@@ -3124,7 +3169,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>272</v>
       </c>
@@ -3132,7 +3177,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>271</v>
       </c>
@@ -3140,7 +3185,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>274</v>
       </c>
@@ -3148,7 +3193,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>318</v>
       </c>
@@ -3156,7 +3201,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>319</v>
       </c>
@@ -3164,7 +3209,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>320</v>
       </c>
@@ -3178,7 +3223,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>275</v>
       </c>
@@ -3186,7 +3231,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>273</v>
       </c>
@@ -3194,12 +3239,158 @@
         <v>323</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>253</v>
       </c>
       <c r="B38" t="s">
         <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>378</v>
+      </c>
+      <c r="B10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>381</v>
+      </c>
+      <c r="B15" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>